<commit_message>
GTEM Import/Export Power. Improvements to Domoticz
</commit_message>
<xml_diff>
--- a/Code/GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz/Energy Setpoint Calculator GTEM Bring-Up Only.xlsx
+++ b/Code/GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz/Energy Setpoint Calculator GTEM Bring-Up Only.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DitroniX\Projects\_DitroniX\GTEM (Grid Tie Energy Monitor)\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DitroniX\Projects\_DitroniX\GTEM (Grid Tie Energy Monitor)\Code\GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07AECE3-31B3-4160-A4EC-26136BCE4B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1818519-BF8D-4AB6-A5A2-B9407077E14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76680" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="GTEM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="GL">Sheet1!$B$24</definedName>
-    <definedName name="IB">Sheet1!$B$23</definedName>
-    <definedName name="Iratio">Sheet1!$B$2</definedName>
-    <definedName name="MC">Sheet1!$B$27</definedName>
-    <definedName name="UN">Sheet1!$B$22</definedName>
-    <definedName name="VL">Sheet1!$B$25</definedName>
-    <definedName name="Vratio">Sheet1!$B$1</definedName>
-    <definedName name="VU">Sheet1!$B$26</definedName>
+    <definedName name="GL">GTEM!$B$24</definedName>
+    <definedName name="IB">GTEM!$B$23</definedName>
+    <definedName name="Iratio">GTEM!$B$2</definedName>
+    <definedName name="MC">GTEM!$B$27</definedName>
+    <definedName name="UN">GTEM!$B$22</definedName>
+    <definedName name="VL">GTEM!$B$25</definedName>
+    <definedName name="Vratio">GTEM!$B$1</definedName>
+    <definedName name="VU">GTEM!$B$26</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -235,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="113">
   <si>
     <t>Voltage ratio</t>
   </si>
@@ -848,6 +857,54 @@
   <si>
     <t>Impulse converter</t>
   </si>
+  <si>
+    <t>Example Values</t>
+  </si>
+  <si>
+    <t>Based on a YHDC SCT-013 100A/50mA Current Transformer</t>
+  </si>
+  <si>
+    <t>  _lgain = 0x1D39; // Use XLS to calculate these values, PL CONSTANT. Examples: 0x1D39;</t>
+  </si>
+  <si>
+    <t>  _igain = 0x7160; // Use XLS to calculate these CURRENT GAIN values. Examples:  0x7160;</t>
+  </si>
+  <si>
+    <t>  _crc1 = 0xAE70;  // Important! Run this application, then take auto CRC1 calculated values and update here. Examples: 0xAE70</t>
+  </si>
+  <si>
+    <t>8V AC RMS In</t>
+  </si>
+  <si>
+    <t>12V AC RMS In</t>
+  </si>
+  <si>
+    <t>Dave Williams, DitroniX</t>
+  </si>
+  <si>
+    <t>The above example values are what I have used on GTEM to test.   Based on YHDC SCT-013 100A/50mA Current Transformer and DAT01A Mains Transformer</t>
+  </si>
+  <si>
+    <t>These WILL vary from one setup to another due to tolerances or the components, clamp and transformer.</t>
+  </si>
+  <si>
+    <t>Will require CRC2 to be updated (GTEM-1_Defaults)</t>
+  </si>
+  <si>
+    <t>Will require CRC1 to be updated (GTEM-1_Defaults)</t>
+  </si>
+  <si>
+    <t>  _crc2 = 0xDC3E;  // Important! Run this application, then take auto CRC2 calculated values and update here.  Examples: 8V 0xDC3E | 12V 0x51AF or 0xF24C</t>
+  </si>
+  <si>
+    <t>  _crc2 = 0xFC4C;  // Important! Run this application, then take auto CRC2 calculated values and update here.  Examples: 8V 0xDC3E | 12V 0x51AF or 0xF24C</t>
+  </si>
+  <si>
+    <t>  _ugain = 0xA028; // Use XLS to calculate these VOLTAGE RMS values. Examples: 8V 0xA028 | 12V 0x9F9A or 0x9E38</t>
+  </si>
+  <si>
+    <t>  _ugain = 0x9F37; // Use XLS to calculate these VOLTAGE RMS values. Examples: 8V 0xA028 | 12V 0x9F9A or 0x9E38</t>
+  </si>
 </sst>
 </file>
 
@@ -856,7 +913,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,16 +988,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Cambia Math"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Cambia Math"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,6 +1029,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1029,7 +1115,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1066,11 +1152,29 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
@@ -3367,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3377,7 +3481,7 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18">
@@ -3448,12 +3552,12 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="9" t="str">
         <f>LEFT(B5,FIND(":",B5)-1)</f>
         <v>100</v>
@@ -3483,12 +3587,12 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="9" t="str">
         <f t="shared" ref="F6:F12" si="0">LEFT(B6,FIND(":",B6)-1)</f>
         <v>10</v>
@@ -3515,12 +3619,12 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3533,12 +3637,12 @@
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
@@ -3551,12 +3655,12 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3569,12 +3673,12 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3587,12 +3691,12 @@
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3605,12 +3709,12 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0010</v>
@@ -3843,7 +3947,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3877,7 +3981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:18">
       <c r="A49" s="10" t="s">
         <v>51</v>
       </c>
@@ -3891,7 +3995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -3905,10 +4009,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:18">
       <c r="B51" s="10"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:18">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -3920,7 +4024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="18">
+    <row r="53" spans="1:18" ht="18">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -3944,7 +4048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="18">
+    <row r="54" spans="1:18" ht="18">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -3961,7 +4065,7 @@
         <v>0101</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:18">
       <c r="A55" s="8" t="s">
         <v>23</v>
       </c>
@@ -3970,191 +4074,278 @@
         <v>0x1D39</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:18">
       <c r="B56" s="10"/>
     </row>
-    <row r="59" spans="1:12" ht="26.25">
+    <row r="58" spans="1:18">
+      <c r="O58" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="19"/>
+    </row>
+    <row r="59" spans="1:18" ht="26.25">
       <c r="A59" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="O59" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B60" s="16">
-        <v>159.80000000000001</v>
+        <v>159.1</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="K60">
+      <c r="J60">
         <f>B60/B62</f>
-        <v>6.0530303030303031E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>6.0265151515151516E-3</v>
+      </c>
+      <c r="O60" s="25">
+        <v>158.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B61" s="16">
-        <v>248.7</v>
+        <v>244.1</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="E61" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E61" s="17"/>
+      <c r="J61">
+        <f>B61*Vratio</f>
+        <v>0.24324862979571499</v>
+      </c>
       <c r="K61">
-        <f>B61*Vratio</f>
-        <v>0.24783258594917787</v>
-      </c>
-      <c r="L61">
-        <f>K61/K60</f>
-        <v>40.943556126772812</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="18">
+        <f>J61/J60</f>
+        <v>40.363066163462449</v>
+      </c>
+      <c r="O61" s="25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="18">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B62" s="10">
         <v>26400</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" s="22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="O62" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="O63" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="O64" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="O65" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B66" s="10">
         <f>INT(B62*B61/B60)</f>
-        <v>41086</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>40504</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B67" s="7" t="str">
         <f>"0x"&amp;DEC2HEX(B66,4)</f>
-        <v>0xA07E</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>0x9E38</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="O67" s="17"/>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="16">
-        <v>10</v>
+        <v>1.6</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="1:8">
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="16">
-        <v>10</v>
+        <v>1.486</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="E70" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" ht="18">
+      <c r="O70" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="18">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="10">
         <v>31251</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" s="22" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="O71" s="25">
+        <v>159.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="O72" s="25">
+        <v>244.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
+      <c r="O73" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="O74" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B75" s="10">
         <f>INT(B71*B70/B69)</f>
-        <v>31251</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>29024</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="O75" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B76" s="7" t="str">
         <f>"0x"&amp;DEC2HEX(B75,4)</f>
-        <v>0x7A13</v>
-      </c>
-      <c r="E76" t="s">
+        <v>0x7160</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J76" t="s">
         <v>91</v>
       </c>
-      <c r="G76" t="s">
+      <c r="L76" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H76">
+      <c r="M76" s="24">
         <f>INT(3*B75/2^16*2^8)</f>
-        <v>366</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="H77" t="str">
-        <f>DEC2HEX(H76)</f>
-        <v>16E</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>340</v>
+      </c>
+      <c r="O76" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="L77" s="24"/>
+      <c r="M77" s="24" t="str">
+        <f>DEC2HEX(M76)</f>
+        <v>154</v>
+      </c>
+      <c r="O77" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="O79" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="O80" s="26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22">
+      <c r="O81" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="26.25">
+    <row r="86" spans="1:22" ht="26.25">
       <c r="A86" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="V86" s="18"/>
+    </row>
+    <row r="87" spans="1:22">
       <c r="A87" s="1" t="s">
         <v>69</v>
       </c>
@@ -4164,20 +4355,22 @@
       <c r="C87" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="V87" s="18"/>
+    </row>
+    <row r="88" spans="1:22">
       <c r="A88" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B88" s="15">
         <f>B66</f>
-        <v>41086</v>
+        <v>40504</v>
       </c>
       <c r="C88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="V88" s="18"/>
+    </row>
+    <row r="89" spans="1:22">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -4187,23 +4380,27 @@
       <c r="C89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="V89" s="18"/>
+    </row>
+    <row r="90" spans="1:22">
+      <c r="V90" s="18"/>
+    </row>
+    <row r="94" spans="1:22">
       <c r="A94" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B94" s="10">
         <f>INT(100*B87*SQRT(2)*B89/(4*B88/32768))</f>
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>6183</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22">
       <c r="A95" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B95" s="7" t="str">
         <f>"0x"&amp;DEC2HEX(B94,4)</f>
-        <v>0x17D0</v>
+        <v>0x1827</v>
       </c>
     </row>
   </sheetData>
@@ -4248,28 +4445,4 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
AT24C64 EEPROM Enabled.  Automatic CRC Update Upon Calibration Default Changes.
</commit_message>
<xml_diff>
--- a/Code/GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz/Energy Setpoint Calculator GTEM Bring-Up Only.xlsx
+++ b/Code/GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz/Energy Setpoint Calculator GTEM Bring-Up Only.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DitroniX\Projects\_DitroniX\GTEM (Grid Tie Energy Monitor)\Code\GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DitroniX\Projects\_DitroniX\_Domoticz\Code\GTEM-1_Test_ATM90E26_Basic_Calibration-Domoticz-DW-House\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1818519-BF8D-4AB6-A5A2-B9407077E14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAA19EA-E66B-4D29-824C-800BA973AAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="76680" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t>Voltage ratio</t>
   </si>
@@ -891,9 +891,6 @@
     <t>Will require CRC2 to be updated (GTEM-1_Defaults)</t>
   </si>
   <si>
-    <t>Will require CRC1 to be updated (GTEM-1_Defaults)</t>
-  </si>
-  <si>
     <t>  _crc2 = 0xDC3E;  // Important! Run this application, then take auto CRC2 calculated values and update here.  Examples: 8V 0xDC3E | 12V 0x51AF or 0xF24C</t>
   </si>
   <si>
@@ -904,6 +901,12 @@
   </si>
   <si>
     <t>  _ugain = 0x9F37; // Use XLS to calculate these VOLTAGE RMS values. Examples: 8V 0xA028 | 12V 0x9F9A or 0x9E38</t>
+  </si>
+  <si>
+    <t>Actual Current</t>
+  </si>
+  <si>
+    <t>Temp</t>
   </si>
 </sst>
 </file>
@@ -3472,7 +3475,7 @@
   <dimension ref="A1:V95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+      <selection activeCell="AC42" sqref="AC42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4089,6 +4092,9 @@
       <c r="A59" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="I59" s="24" t="s">
+        <v>113</v>
+      </c>
       <c r="O59" s="22" t="s">
         <v>102</v>
       </c>
@@ -4106,6 +4112,9 @@
       <c r="E60" s="22" t="s">
         <v>67</v>
       </c>
+      <c r="I60" s="24">
+        <v>159.1</v>
+      </c>
       <c r="J60">
         <f>B60/B62</f>
         <v>6.0265151515151516E-3</v>
@@ -4127,6 +4136,9 @@
       <c r="E61" s="23" t="s">
         <v>70</v>
       </c>
+      <c r="I61" s="24">
+        <v>244.1</v>
+      </c>
       <c r="J61">
         <f>B61*Vratio</f>
         <v>0.24324862979571499</v>
@@ -4149,21 +4161,25 @@
       <c r="E62" s="22" t="s">
         <v>73</v>
       </c>
+      <c r="I62" s="24"/>
       <c r="O62" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:18">
+      <c r="I63" s="24"/>
       <c r="O63" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:18">
+      <c r="I64" s="24"/>
       <c r="O64" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:15">
+      <c r="I65" s="24"/>
       <c r="O65" s="17" t="s">
         <v>101</v>
       </c>
@@ -4176,8 +4192,9 @@
         <f>INT(B62*B61/B60)</f>
         <v>40504</v>
       </c>
+      <c r="I66" s="24"/>
       <c r="O66" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:15">
@@ -4191,7 +4208,11 @@
       <c r="E67" s="21" t="s">
         <v>107</v>
       </c>
+      <c r="I67" s="24"/>
       <c r="O67" s="17"/>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="I68" s="24"/>
     </row>
     <row r="69" spans="1:15">
       <c r="A69" s="1" t="s">
@@ -4206,6 +4227,9 @@
       <c r="E69" s="22" t="s">
         <v>67</v>
       </c>
+      <c r="I69" s="24">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="70" spans="1:15">
       <c r="A70" s="1" t="s">
@@ -4218,7 +4242,10 @@
         <v>4</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>70</v>
+        <v>112</v>
+      </c>
+      <c r="I70" s="24">
+        <v>1.486</v>
       </c>
       <c r="O70" s="23" t="s">
         <v>103</v>
@@ -4250,7 +4277,7 @@
     </row>
     <row r="74" spans="1:15">
       <c r="O74" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -4277,7 +4304,7 @@
         <v>0x7160</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J76" t="s">
         <v>91</v>
@@ -4300,7 +4327,7 @@
         <v>154</v>
       </c>
       <c r="O77" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:15">

</xml_diff>